<commit_message>
Updated Power consumption estimate
</commit_message>
<xml_diff>
--- a/Documents/CubeSat_Sub-Systems/Power/Data/CubeSat Power Data.xlsx
+++ b/Documents/CubeSat_Sub-Systems/Power/Data/CubeSat Power Data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t xml:space="preserve">Company </t>
   </si>
@@ -133,12 +133,6 @@
     <t>HASP</t>
   </si>
   <si>
-    <t>Radio</t>
-  </si>
-  <si>
-    <t>Antenna</t>
-  </si>
-  <si>
     <t>GPS</t>
   </si>
   <si>
@@ -148,16 +142,28 @@
     <t>Attitude</t>
   </si>
   <si>
-    <t xml:space="preserve">Rule of thumb power from solar </t>
-  </si>
-  <si>
-    <t>P=.60*Power(one panel)</t>
-  </si>
-  <si>
     <t>ON-Time(min)</t>
   </si>
   <si>
     <t>Energy Used (Wh)</t>
+  </si>
+  <si>
+    <t>Radio/Antenna</t>
+  </si>
+  <si>
+    <t>OBC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>Solar 1 side</t>
+  </si>
+  <si>
+    <t>Power in - out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Battery wattage to be determined </t>
   </si>
 </sst>
 </file>
@@ -568,7 +574,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A10"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -924,21 +930,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -946,13 +952,13 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -960,44 +966,81 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6">
+        <v>1.15E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9">
+        <f>SUM(B2:B7)</f>
+        <v>7.500515</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="B12">
+        <v>6.62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <f>B12-(B9+B11)</f>
+        <v>-0.88051499999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>